<commit_message>
docs: requirement list, use case description, use case diagram final v1.1
</commit_message>
<xml_diff>
--- a/SE_Team2_Requirement_list_final.xlsx
+++ b/SE_Team2_Requirement_list_final.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\SE_Team2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C06CF8F1-90B8-437E-85CA-EE2D173A447E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F6D99B2-2A6F-40BD-87CD-8D220853B870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2B9A1A4C-40C9-46E0-9101-937DFF5848E6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2B9A1A4C-40C9-46E0-9101-937DFF5848E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="62">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -200,9 +200,6 @@
     <t xml:space="preserve">관리자는 등록된 자전거 리스트를 조회할 수 있다. </t>
   </si>
   <si>
-    <t>관리자는 자전거 리스트 조회 화면에서 원하는 자전거 항목을 선택해서 상세내용(자전거 ID, 자전거 제품명, 유형(일반/전기), 소속 대여소, 상태(사용 가능/수리 중))을 볼 수 있다.</t>
-  </si>
-  <si>
     <t>관리자는 자전거 리스트 조회 화면에서 특정 자전거 항목을 삭제할 수 있다.</t>
   </si>
   <si>
@@ -224,13 +221,60 @@
   <si>
     <t>Use Case(s)</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Use case Diagram, Requirement list, Use case Description 최종본 작성 (로그인, 로그아웃, 자전거 대여소 등록, 자전거 대여소 리스트 조회, 대여소 상세 정보 조회, 대여소 삭제)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Github Repository 관리 및 제출 파일 검토</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Use case Diagram, Requirement list 의견 조율 및 최종 병합</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Use case Diagram, Requirement list, Use case Description 최종본 작성 (자전거 등록, 등록된 자전거 리스트 조회, 자전거 상세 정보 조회, 자전거 삭제, 자전거 대여 정보 조회, 지역별 정렬 기준 변경, 대여 금액 및 횟수 조회, 대여 기간 단위 변경)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Use case Diagram, Requirement list 초안 작성 (전체적인 workflow 확인)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Use case Diagram workflow 검토: 자전거 반납 및 요금 조회, 식당 예약 시스템</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Use case Diagram workflow 검토: 대여 금액 및 횟수 조회와 대여 기간 단위 변경</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Use case Diagram workflow 검토: 즉시 대여, 예약 대기 및 문자 발송 시스템</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>소프트웨어공학 2팀</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Use case Diagram, Requirement list, Use case Description 최종본 작성 (대여 자전거 조회, 예약 대기 조회, 요금 조회, 대여 기록 조회, 대여소 정렬 기준 변겅, 대여 기록 삭제)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Use case Diagram, Requirement list, Use case Description 최종본 작성 (회원가입, 대여소 리스트 검색, 대여소 상세정보 조회, 즉시 대여, 예약 대기, 회원 탈퇴)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>관리자는 자전거 리스트 조회 화면에서 원하는 자전거 항목을 선택해서 상세내용(자전거 ID, 자전거 제품명, 유형(일반/전기), 소속 대여소, 상태(사용 가능/수리 중))화면을 볼 수 있다.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -263,6 +307,15 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -272,7 +325,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -362,13 +415,95 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -393,12 +528,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -429,6 +558,39 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -440,6 +602,21 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -775,10 +952,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D32EF711-E41E-4776-BBB7-C6C14271EF27}">
-  <dimension ref="A1:C183"/>
+  <dimension ref="A1:C196"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -787,328 +964,405 @@
     <col min="2" max="3" width="63.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:3" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="18">
+        <v>35427</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="20"/>
+    </row>
+    <row r="2" spans="1:3" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="25"/>
+    </row>
+    <row r="3" spans="1:3" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="22"/>
+      <c r="B3" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="27"/>
+    </row>
+    <row r="4" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="23"/>
+      <c r="B4" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="34"/>
+    </row>
+    <row r="5" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="25"/>
+    </row>
+    <row r="6" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="22"/>
+      <c r="B6" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="27"/>
+    </row>
+    <row r="7" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="22"/>
+      <c r="B7" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="27"/>
+    </row>
+    <row r="8" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="23"/>
+      <c r="B8" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" s="34"/>
+    </row>
+    <row r="9" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="25"/>
+    </row>
+    <row r="10" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="22"/>
+      <c r="B10" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="27"/>
+    </row>
+    <row r="11" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="23"/>
+      <c r="B11" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="34"/>
+    </row>
+    <row r="12" spans="1:3" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="27"/>
+    </row>
+    <row r="13" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="22"/>
+      <c r="B13" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="27"/>
+    </row>
+    <row r="14" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="23"/>
+      <c r="B14" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" s="34"/>
+    </row>
+    <row r="15" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="28"/>
+      <c r="C15" s="28"/>
+    </row>
+    <row r="16" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B16" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="19" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="10"/>
-      <c r="B2" s="22" t="s">
+      <c r="C16" s="17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="8"/>
+      <c r="B17" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="23"/>
-    </row>
-    <row r="3" spans="1:3" ht="50.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
+      <c r="C17" s="32"/>
+    </row>
+    <row r="18" spans="1:3" ht="50.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="3">
         <v>1</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B18" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C18" s="14" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="4">
+    <row r="19" spans="1:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="4">
         <v>2</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B19" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C19" s="15" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="4">
+    <row r="20" spans="1:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="4">
         <v>3</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B20" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C20" s="15" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="4">
+    <row r="21" spans="1:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="4">
         <v>4</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B21" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C21" s="15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="4">
+    <row r="22" spans="1:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="4">
         <v>5</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B22" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C22" s="15" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="4">
+    <row r="23" spans="1:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="4">
         <v>6</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B23" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C23" s="15" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="13"/>
-      <c r="B9" s="20" t="s">
+    <row r="24" spans="1:3" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="11"/>
+      <c r="B24" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="21"/>
-    </row>
-    <row r="10" spans="1:3" ht="50.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="11">
+      <c r="C24" s="30"/>
+    </row>
+    <row r="25" spans="1:3" ht="50.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="9">
         <v>7</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B25" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C25" s="10" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="6">
-        <v>8</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="6">
-        <v>9</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="6">
-        <v>10</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="13"/>
-      <c r="B14" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="21"/>
-    </row>
-    <row r="15" spans="1:3" ht="100.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="11">
-        <v>11</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="63" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="6">
-        <v>12</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="6">
-        <v>13</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="6">
-        <v>14</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C18" s="15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="13"/>
-      <c r="B19" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="C19" s="21"/>
-    </row>
-    <row r="20" spans="1:3" ht="50.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="11">
-        <v>15</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="6">
-        <v>16</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="6">
-        <v>17</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="6">
-        <v>18</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="6">
-        <v>19</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="6">
-        <v>20</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="6">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>39</v>
+        <v>16</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="6">
+        <v>9</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="6">
+        <v>10</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B27" s="1" t="s">
+    </row>
+    <row r="29" spans="1:3" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="11"/>
+      <c r="B29" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" s="30"/>
+    </row>
+    <row r="30" spans="1:3" ht="50.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="9">
+        <v>11</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="6">
+        <v>12</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="6">
+        <v>13</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="6">
+        <v>14</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="11"/>
+      <c r="B34" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C34" s="37"/>
+    </row>
+    <row r="35" spans="1:3" ht="50.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="9">
+        <v>15</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="6">
+        <v>16</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="6">
+        <v>17</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="6">
+        <v>18</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="6">
+        <v>19</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="6">
+        <v>20</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="6">
+        <v>21</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="6">
+        <v>22</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="9"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-    </row>
-    <row r="29" spans="1:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="9"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-    </row>
-    <row r="30" spans="1:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="9"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-    </row>
-    <row r="31" spans="1:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="9"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-    </row>
-    <row r="32" spans="1:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="9"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
-    </row>
-    <row r="33" ht="50.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="34" ht="50.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="35" ht="50.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="36" ht="50.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="37" ht="50.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="38" ht="50.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="39" ht="50.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="40" ht="50.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="41" ht="50.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="42" ht="50.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="43" ht="50.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="44" ht="50.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="45" ht="50.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="46" ht="50.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="47" ht="50.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="48" ht="50.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="1:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="44" spans="1:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="1:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="46" spans="1:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="1:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="48" spans="1:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="49" ht="50.1" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="50" ht="50.1" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="51" ht="50.1" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1244,12 +1498,44 @@
     <row r="181" ht="50.1" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="182" ht="50.1" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="183" ht="50.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="184" ht="50.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="185" ht="50.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="186" ht="50.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="187" ht="50.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="188" ht="50.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="189" ht="50.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="190" ht="50.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="191" ht="50.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="192" ht="50.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="193" ht="50.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="194" ht="50.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="195" ht="50.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="196" ht="50.1" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B2:C2"/>
+  <mergeCells count="23">
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B29:C29"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B8:C8"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>